<commit_message>
fixed price import and fixed cyclical csv-imports, adopted constraints for charging / discharging storage
</commit_message>
<xml_diff>
--- a/CoSES/02_Interface_Server/parametrization.xlsx
+++ b/CoSES/02_Interface_Server/parametrization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="1" r:id="rId1"/>
@@ -3807,8 +3807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4231,7 +4231,7 @@
         <v>56</v>
       </c>
       <c r="D32">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -4245,7 +4245,7 @@
         <v>46</v>
       </c>
       <c r="D33">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -4294,7 +4294,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4689,7 +4689,7 @@
         <v>56</v>
       </c>
       <c r="D32">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
@@ -4703,7 +4703,7 @@
         <v>46</v>
       </c>
       <c r="D33">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -4751,8 +4751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>